<commit_message>
Atualização de dados: 23/07/2025
Atualização de dados: 23/07/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A82A09-2DDA-482F-9595-9AF67C24F1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47526B9-92DA-422E-BBB8-93791AE322A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6172" uniqueCount="6127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6174" uniqueCount="6129">
   <si>
     <t>Fecha</t>
   </si>
@@ -18369,10 +18369,16 @@
     <t>2025/07/20</t>
   </si>
   <si>
+    <t>2025/07/21</t>
+  </si>
+  <si>
+    <t>2025/07/22</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República lunes, 21 de julio de 2025 8:20:32 a. m.</t>
+    <t>Descargado de sistema del Banco de la República miércoles, 23 de julio de 2025 10:14:56 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -18788,10 +18794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6090"/>
+  <dimension ref="A1:B6092"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67499,15 +67505,31 @@
       <c r="A6088" t="s">
         <v>6117</v>
       </c>
+      <c r="B6088" s="1">
+        <v>4679.7135399999997</v>
+      </c>
     </row>
     <row r="6089" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6089" t="s">
-        <v>6117</v>
+        <v>6118</v>
+      </c>
+      <c r="B6089" s="1">
+        <v>4720.1976299999997</v>
       </c>
     </row>
     <row r="6090" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6090" t="s">
-        <v>6118</v>
+        <v>6119</v>
+      </c>
+    </row>
+    <row r="6091" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6091" t="s">
+        <v>6119</v>
+      </c>
+    </row>
+    <row r="6092" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6092" t="s">
+        <v>6120</v>
       </c>
     </row>
   </sheetData>
@@ -67533,19 +67555,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6119</v>
+        <v>6121</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6120</v>
+        <v>6122</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6121</v>
+        <v>6123</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6122</v>
+        <v>6124</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6123</v>
+        <v>6125</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67556,13 +67578,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67573,13 +67595,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67590,13 +67612,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67607,13 +67629,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67624,13 +67646,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67641,13 +67663,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67658,13 +67680,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67675,13 +67697,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67692,13 +67714,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67709,13 +67731,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67726,13 +67748,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67743,13 +67765,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67760,13 +67782,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67777,13 +67799,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67794,13 +67816,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6124</v>
+        <v>6126</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6125</v>
+        <v>6127</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6126</v>
+        <v>6128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 20/08/2025
Atualização de arquivo: 20/08/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFD4F35-6151-4805-BC7F-420AB0820539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7A91F4-1878-4AD7-9FB2-C6E736A87F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6200" uniqueCount="6155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6202" uniqueCount="6157">
   <si>
     <t>Fecha</t>
   </si>
@@ -18453,10 +18453,16 @@
     <t>2025/08/17</t>
   </si>
   <si>
+    <t>2025/08/18</t>
+  </si>
+  <si>
+    <t>2025/08/19</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República lunes, 18 de agosto de 2025 8:10:02 a. m.</t>
+    <t>Descargado de sistema del Banco de la República miércoles, 20 de agosto de 2025 9:17:45 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -18872,10 +18878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6118"/>
+  <dimension ref="A1:B6120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67807,15 +67813,31 @@
       <c r="A6116" t="s">
         <v>6145</v>
       </c>
+      <c r="B6116" s="1">
+        <v>4688.2424899999996</v>
+      </c>
     </row>
     <row r="6117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6117" t="s">
-        <v>6145</v>
+        <v>6146</v>
+      </c>
+      <c r="B6117" s="1">
+        <v>4691.4578899999997</v>
       </c>
     </row>
     <row r="6118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6118" t="s">
-        <v>6146</v>
+        <v>6147</v>
+      </c>
+    </row>
+    <row r="6119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6119" t="s">
+        <v>6147</v>
+      </c>
+    </row>
+    <row r="6120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6120" t="s">
+        <v>6148</v>
       </c>
     </row>
   </sheetData>
@@ -67841,19 +67863,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6147</v>
+        <v>6149</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6148</v>
+        <v>6150</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6149</v>
+        <v>6151</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6150</v>
+        <v>6152</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6151</v>
+        <v>6153</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67864,13 +67886,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67881,13 +67903,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67898,13 +67920,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67915,13 +67937,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67932,13 +67954,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67949,13 +67971,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67966,13 +67988,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67983,13 +68005,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68000,13 +68022,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68017,13 +68039,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68034,13 +68056,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68051,13 +68073,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68068,13 +68090,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68085,13 +68107,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68102,13 +68124,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6152</v>
+        <v>6154</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6153</v>
+        <v>6155</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6154</v>
+        <v>6156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 25/08/2025
Atualização de arquivo: 25/08/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7A91F4-1878-4AD7-9FB2-C6E736A87F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6F6A26-184D-4F32-93EC-1E9DF6083656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6202" uniqueCount="6157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6207" uniqueCount="6162">
   <si>
     <t>Fecha</t>
   </si>
@@ -18459,10 +18459,25 @@
     <t>2025/08/19</t>
   </si>
   <si>
+    <t>2025/08/20</t>
+  </si>
+  <si>
+    <t>2025/08/21</t>
+  </si>
+  <si>
+    <t>2025/08/22</t>
+  </si>
+  <si>
+    <t>2025/08/23</t>
+  </si>
+  <si>
+    <t>2025/08/24</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República miércoles, 20 de agosto de 2025 9:17:45 a. m.</t>
+    <t>Descargado de sistema del Banco de la República lunes, 25 de agosto de 2025 7:01:23 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -18878,10 +18893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6120"/>
+  <dimension ref="A1:B6125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67829,15 +67844,55 @@
       <c r="A6118" t="s">
         <v>6147</v>
       </c>
+      <c r="B6118" s="1">
+        <v>4707.6766399999997</v>
+      </c>
     </row>
     <row r="6119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6119" t="s">
-        <v>6147</v>
+        <v>6148</v>
+      </c>
+      <c r="B6119" s="1">
+        <v>4676.23369</v>
       </c>
     </row>
     <row r="6120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6120" t="s">
-        <v>6148</v>
+        <v>6149</v>
+      </c>
+      <c r="B6120" s="1">
+        <v>4727.2521200000001</v>
+      </c>
+    </row>
+    <row r="6121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6121" t="s">
+        <v>6150</v>
+      </c>
+      <c r="B6121" s="1">
+        <v>4697.3946599999999</v>
+      </c>
+    </row>
+    <row r="6122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6122" t="s">
+        <v>6151</v>
+      </c>
+      <c r="B6122" s="1">
+        <v>4697.3946599999999</v>
+      </c>
+    </row>
+    <row r="6123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6123" t="s">
+        <v>6152</v>
+      </c>
+    </row>
+    <row r="6124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6124" t="s">
+        <v>6152</v>
+      </c>
+    </row>
+    <row r="6125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6125" t="s">
+        <v>6153</v>
       </c>
     </row>
   </sheetData>
@@ -67863,19 +67918,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6149</v>
+        <v>6154</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6150</v>
+        <v>6155</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6151</v>
+        <v>6156</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6152</v>
+        <v>6157</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6153</v>
+        <v>6158</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67886,13 +67941,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67903,13 +67958,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67920,13 +67975,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67937,13 +67992,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67954,13 +68009,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67971,13 +68026,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67988,13 +68043,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68005,13 +68060,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68022,13 +68077,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68039,13 +68094,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68056,13 +68111,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68073,13 +68128,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68090,13 +68145,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68107,13 +68162,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68124,13 +68179,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6154</v>
+        <v>6159</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6155</v>
+        <v>6160</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6156</v>
+        <v>6161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 28/08/2025
Atualização de arquivo: 28/08/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6F6A26-184D-4F32-93EC-1E9DF6083656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DC472B-DC2C-4E89-A462-698E82904F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6207" uniqueCount="6162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6210" uniqueCount="6165">
   <si>
     <t>Fecha</t>
   </si>
@@ -18474,10 +18474,19 @@
     <t>2025/08/24</t>
   </si>
   <si>
+    <t>2025/08/25</t>
+  </si>
+  <si>
+    <t>2025/08/26</t>
+  </si>
+  <si>
+    <t>2025/08/27</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República lunes, 25 de agosto de 2025 7:01:23 a. m.</t>
+    <t>Descargado de sistema del Banco de la República jueves, 28 de agosto de 2025 7:12:40 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -18893,10 +18902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6125"/>
+  <dimension ref="A1:B6128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F7" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67884,15 +67893,39 @@
       <c r="A6123" t="s">
         <v>6152</v>
       </c>
+      <c r="B6123" s="1">
+        <v>4686.1702999999998</v>
+      </c>
     </row>
     <row r="6124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6124" t="s">
-        <v>6152</v>
+        <v>6153</v>
+      </c>
+      <c r="B6124" s="1">
+        <v>4681.9245700000001</v>
       </c>
     </row>
     <row r="6125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6125" t="s">
-        <v>6153</v>
+        <v>6154</v>
+      </c>
+      <c r="B6125" s="1">
+        <v>4688.80044</v>
+      </c>
+    </row>
+    <row r="6126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6126" t="s">
+        <v>6155</v>
+      </c>
+    </row>
+    <row r="6127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6127" t="s">
+        <v>6155</v>
+      </c>
+    </row>
+    <row r="6128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6128" t="s">
+        <v>6156</v>
       </c>
     </row>
   </sheetData>
@@ -67918,19 +67951,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6154</v>
+        <v>6157</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6155</v>
+        <v>6158</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6156</v>
+        <v>6159</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6157</v>
+        <v>6160</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6158</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67941,13 +67974,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67958,13 +67991,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67975,13 +68008,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67992,13 +68025,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68009,13 +68042,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68026,13 +68059,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68043,13 +68076,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68060,13 +68093,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68077,13 +68110,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68094,13 +68127,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68111,13 +68144,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68128,13 +68161,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68145,13 +68178,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68162,13 +68195,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68179,13 +68212,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6159</v>
+        <v>6162</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6160</v>
+        <v>6163</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 17/09/2025
Atualização de arquivo: 17/09/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DC472B-DC2C-4E89-A462-698E82904F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D99D24D-8CBE-40CE-8F49-633ED1F16351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6210" uniqueCount="6165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6230" uniqueCount="6185">
   <si>
     <t>Fecha</t>
   </si>
@@ -18483,10 +18483,70 @@
     <t>2025/08/27</t>
   </si>
   <si>
+    <t>2025/08/28</t>
+  </si>
+  <si>
+    <t>2025/08/29</t>
+  </si>
+  <si>
+    <t>2025/08/30</t>
+  </si>
+  <si>
+    <t>2025/08/31</t>
+  </si>
+  <si>
+    <t>2025/09/01</t>
+  </si>
+  <si>
+    <t>2025/09/02</t>
+  </si>
+  <si>
+    <t>2025/09/03</t>
+  </si>
+  <si>
+    <t>2025/09/04</t>
+  </si>
+  <si>
+    <t>2025/09/05</t>
+  </si>
+  <si>
+    <t>2025/09/06</t>
+  </si>
+  <si>
+    <t>2025/09/07</t>
+  </si>
+  <si>
+    <t>2025/09/08</t>
+  </si>
+  <si>
+    <t>2025/09/09</t>
+  </si>
+  <si>
+    <t>2025/09/10</t>
+  </si>
+  <si>
+    <t>2025/09/11</t>
+  </si>
+  <si>
+    <t>2025/09/12</t>
+  </si>
+  <si>
+    <t>2025/09/13</t>
+  </si>
+  <si>
+    <t>2025/09/14</t>
+  </si>
+  <si>
+    <t>2025/09/15</t>
+  </si>
+  <si>
+    <t>2025/09/16</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República jueves, 28 de agosto de 2025 7:12:40 a. m.</t>
+    <t>Descargado de sistema del Banco de la República miércoles, 17 de septiembre de 2025 7:59:40 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -18902,10 +18962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6128"/>
+  <dimension ref="A1:B6148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F6:F7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67917,15 +67977,175 @@
       <c r="A6126" t="s">
         <v>6155</v>
       </c>
+      <c r="B6126" s="1">
+        <v>4728.8515799999996</v>
+      </c>
     </row>
     <row r="6127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6127" t="s">
-        <v>6155</v>
+        <v>6156</v>
+      </c>
+      <c r="B6127" s="1">
+        <v>4704.3448399999997</v>
       </c>
     </row>
     <row r="6128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6128" t="s">
-        <v>6156</v>
+        <v>6157</v>
+      </c>
+      <c r="B6128" s="1">
+        <v>4703.5488999999998</v>
+      </c>
+    </row>
+    <row r="6129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6129" t="s">
+        <v>6158</v>
+      </c>
+      <c r="B6129" s="1">
+        <v>4703.5488999999998</v>
+      </c>
+    </row>
+    <row r="6130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6130" t="s">
+        <v>6159</v>
+      </c>
+      <c r="B6130" s="1">
+        <v>4706.1608699999997</v>
+      </c>
+    </row>
+    <row r="6131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6131" t="s">
+        <v>6160</v>
+      </c>
+      <c r="B6131" s="1">
+        <v>4686.6715800000002</v>
+      </c>
+    </row>
+    <row r="6132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6132" t="s">
+        <v>6161</v>
+      </c>
+      <c r="B6132" s="1">
+        <v>4685.1579599999995</v>
+      </c>
+    </row>
+    <row r="6133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6133" t="s">
+        <v>6162</v>
+      </c>
+      <c r="B6133" s="1">
+        <v>4657.3276100000003</v>
+      </c>
+    </row>
+    <row r="6134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6134" t="s">
+        <v>6163</v>
+      </c>
+      <c r="B6134" s="1">
+        <v>4684.1427700000004</v>
+      </c>
+    </row>
+    <row r="6135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6135" t="s">
+        <v>6164</v>
+      </c>
+      <c r="B6135" s="1">
+        <v>4648.7572300000002</v>
+      </c>
+    </row>
+    <row r="6136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6136" t="s">
+        <v>6165</v>
+      </c>
+      <c r="B6136" s="1">
+        <v>4648.7572300000002</v>
+      </c>
+    </row>
+    <row r="6137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6137" t="s">
+        <v>6166</v>
+      </c>
+      <c r="B6137" s="1">
+        <v>4652.1240299999999</v>
+      </c>
+    </row>
+    <row r="6138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6138" t="s">
+        <v>6167</v>
+      </c>
+      <c r="B6138" s="1">
+        <v>4628.4169599999996</v>
+      </c>
+    </row>
+    <row r="6139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6139" t="s">
+        <v>6168</v>
+      </c>
+      <c r="B6139" s="1">
+        <v>4596.1597000000002</v>
+      </c>
+    </row>
+    <row r="6140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6140" t="s">
+        <v>6169</v>
+      </c>
+      <c r="B6140" s="1">
+        <v>4599.2290199999998</v>
+      </c>
+    </row>
+    <row r="6141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6141" t="s">
+        <v>6170</v>
+      </c>
+      <c r="B6141" s="1">
+        <v>4577.25918</v>
+      </c>
+    </row>
+    <row r="6142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6142" t="s">
+        <v>6171</v>
+      </c>
+      <c r="B6142" s="1">
+        <v>4580.84764</v>
+      </c>
+    </row>
+    <row r="6143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6143" t="s">
+        <v>6172</v>
+      </c>
+      <c r="B6143" s="1">
+        <v>4580.84764</v>
+      </c>
+    </row>
+    <row r="6144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6144" t="s">
+        <v>6173</v>
+      </c>
+      <c r="B6144" s="1">
+        <v>4592.9569899999997</v>
+      </c>
+    </row>
+    <row r="6145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6145" t="s">
+        <v>6174</v>
+      </c>
+      <c r="B6145" s="1">
+        <v>4619.3999599999997</v>
+      </c>
+    </row>
+    <row r="6146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6146" t="s">
+        <v>6175</v>
+      </c>
+    </row>
+    <row r="6147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6147" t="s">
+        <v>6175</v>
+      </c>
+    </row>
+    <row r="6148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6148" t="s">
+        <v>6176</v>
       </c>
     </row>
   </sheetData>
@@ -67951,19 +68171,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6157</v>
+        <v>6177</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6158</v>
+        <v>6178</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6159</v>
+        <v>6179</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6160</v>
+        <v>6180</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6161</v>
+        <v>6181</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67974,13 +68194,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -67991,13 +68211,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68008,13 +68228,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68025,13 +68245,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68042,13 +68262,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68059,13 +68279,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68076,13 +68296,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68093,13 +68313,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68110,13 +68330,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68127,13 +68347,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68144,13 +68364,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68161,13 +68381,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68178,13 +68398,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68195,13 +68415,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68212,13 +68432,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6162</v>
+        <v>6182</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6163</v>
+        <v>6183</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6164</v>
+        <v>6184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 22/09/2025
Atualização de arquivo: 22/09/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D99D24D-8CBE-40CE-8F49-633ED1F16351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F346AE-ED12-43C8-AFA5-ADD994A9A194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6230" uniqueCount="6185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6235" uniqueCount="6190">
   <si>
     <t>Fecha</t>
   </si>
@@ -18543,10 +18543,25 @@
     <t>2025/09/16</t>
   </si>
   <si>
+    <t>2025/09/17</t>
+  </si>
+  <si>
+    <t>2025/09/18</t>
+  </si>
+  <si>
+    <t>2025/09/19</t>
+  </si>
+  <si>
+    <t>2025/09/20</t>
+  </si>
+  <si>
+    <t>2025/09/21</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República miércoles, 17 de septiembre de 2025 7:59:40 a. m.</t>
+    <t>Descargado de sistema del Banco de la República lunes, 22 de septiembre de 2025 8:06:05 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -18962,10 +18977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6148"/>
+  <dimension ref="A1:B6153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68137,15 +68152,55 @@
       <c r="A6146" t="s">
         <v>6175</v>
       </c>
+      <c r="B6146" s="1">
+        <v>4600.0752000000002</v>
+      </c>
     </row>
     <row r="6147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6147" t="s">
-        <v>6175</v>
+        <v>6176</v>
+      </c>
+      <c r="B6147" s="1">
+        <v>4569.0997699999998</v>
       </c>
     </row>
     <row r="6148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6148" t="s">
-        <v>6176</v>
+        <v>6177</v>
+      </c>
+      <c r="B6148" s="1">
+        <v>4576.7427100000004</v>
+      </c>
+    </row>
+    <row r="6149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6149" t="s">
+        <v>6178</v>
+      </c>
+      <c r="B6149" s="1">
+        <v>4575.2611999999999</v>
+      </c>
+    </row>
+    <row r="6150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6150" t="s">
+        <v>6179</v>
+      </c>
+      <c r="B6150" s="1">
+        <v>4575.2611999999999</v>
+      </c>
+    </row>
+    <row r="6151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6151" t="s">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="6152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6152" t="s">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="6153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6153" t="s">
+        <v>6181</v>
       </c>
     </row>
   </sheetData>
@@ -68171,19 +68226,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6177</v>
+        <v>6182</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6178</v>
+        <v>6183</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6179</v>
+        <v>6184</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6180</v>
+        <v>6185</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6181</v>
+        <v>6186</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68194,13 +68249,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68211,13 +68266,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68228,13 +68283,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68245,13 +68300,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68262,13 +68317,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68279,13 +68334,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68296,13 +68351,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68313,13 +68368,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68330,13 +68385,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68347,13 +68402,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68364,13 +68419,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68381,13 +68436,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68398,13 +68453,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68415,13 +68470,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68432,13 +68487,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6182</v>
+        <v>6187</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6183</v>
+        <v>6188</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6184</v>
+        <v>6189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 23/09/2025
Atualização de arquivo: 23/09/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F346AE-ED12-43C8-AFA5-ADD994A9A194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA5F98C-F5AB-43A9-BD0D-EA0DBA40D381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6235" uniqueCount="6190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6236" uniqueCount="6191">
   <si>
     <t>Fecha</t>
   </si>
@@ -18558,10 +18558,13 @@
     <t>2025/09/21</t>
   </si>
   <si>
+    <t>2025/09/22</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República lunes, 22 de septiembre de 2025 8:06:05 a. m.</t>
+    <t>Descargado de sistema del Banco de la República martes, 23 de septiembre de 2025 7:23:48 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -18977,10 +18980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6153"/>
+  <dimension ref="A1:B6154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68192,15 +68195,23 @@
       <c r="A6151" t="s">
         <v>6180</v>
       </c>
+      <c r="B6151" s="1">
+        <v>4580.7088599999997</v>
+      </c>
     </row>
     <row r="6152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6152" t="s">
-        <v>6180</v>
+        <v>6181</v>
       </c>
     </row>
     <row r="6153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6153" t="s">
         <v>6181</v>
+      </c>
+    </row>
+    <row r="6154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6154" t="s">
+        <v>6182</v>
       </c>
     </row>
   </sheetData>
@@ -68226,19 +68237,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6182</v>
+        <v>6183</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6183</v>
+        <v>6184</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6184</v>
+        <v>6185</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6185</v>
+        <v>6186</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6186</v>
+        <v>6187</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68249,13 +68260,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68266,13 +68277,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68283,13 +68294,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68300,13 +68311,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68317,13 +68328,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68334,13 +68345,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68351,13 +68362,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68368,13 +68379,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68385,13 +68396,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68402,13 +68413,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68419,13 +68430,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68436,13 +68447,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68453,13 +68464,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68470,13 +68481,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68487,13 +68498,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 25/09/2025
Atualização de arquivo: 25/09/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA5F98C-F5AB-43A9-BD0D-EA0DBA40D381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF2D9EE-B59B-4810-AF35-AF41A6B85DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6236" uniqueCount="6191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6238" uniqueCount="6193">
   <si>
     <t>Fecha</t>
   </si>
@@ -18561,10 +18561,16 @@
     <t>2025/09/22</t>
   </si>
   <si>
+    <t>2025/09/23</t>
+  </si>
+  <si>
+    <t>2025/09/24</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República martes, 23 de septiembre de 2025 7:23:48 a. m.</t>
+    <t>Descargado de sistema del Banco de la República jueves, 25 de septiembre de 2025 8:24:02 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -18980,10 +18986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6154"/>
+  <dimension ref="A1:B6156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68203,15 +68209,31 @@
       <c r="A6152" t="s">
         <v>6181</v>
       </c>
+      <c r="B6152" s="1">
+        <v>4544.0079299999998</v>
+      </c>
     </row>
     <row r="6153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6153" t="s">
-        <v>6181</v>
+        <v>6182</v>
+      </c>
+      <c r="B6153" s="1">
+        <v>4514.7533400000002</v>
       </c>
     </row>
     <row r="6154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6154" t="s">
-        <v>6182</v>
+        <v>6183</v>
+      </c>
+    </row>
+    <row r="6155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6155" t="s">
+        <v>6183</v>
+      </c>
+    </row>
+    <row r="6156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6156" t="s">
+        <v>6184</v>
       </c>
     </row>
   </sheetData>
@@ -68237,19 +68259,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6183</v>
+        <v>6185</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6184</v>
+        <v>6186</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6185</v>
+        <v>6187</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6186</v>
+        <v>6188</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6187</v>
+        <v>6189</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68260,13 +68282,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68277,13 +68299,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68294,13 +68316,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68311,13 +68333,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68328,13 +68350,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68345,13 +68367,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68362,13 +68384,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68379,13 +68401,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68396,13 +68418,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68413,13 +68435,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68430,13 +68452,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68447,13 +68469,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68464,13 +68486,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68481,13 +68503,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68498,13 +68520,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6188</v>
+        <v>6190</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 26/09/2025
Atualização de arquivo: 26/09/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF2D9EE-B59B-4810-AF35-AF41A6B85DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F18A6D-0E1E-483E-9937-A29149E7190C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6238" uniqueCount="6193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6239" uniqueCount="6194">
   <si>
     <t>Fecha</t>
   </si>
@@ -18567,10 +18567,13 @@
     <t>2025/09/24</t>
   </si>
   <si>
+    <t>2025/09/25</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República jueves, 25 de septiembre de 2025 8:24:02 a. m.</t>
+    <t>Descargado de sistema del Banco de la República viernes, 26 de septiembre de 2025 7:31:53 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -18986,10 +18989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6156"/>
+  <dimension ref="A1:B6157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68225,15 +68228,23 @@
       <c r="A6154" t="s">
         <v>6183</v>
       </c>
+      <c r="B6154" s="1">
+        <v>4531.9532300000001</v>
+      </c>
     </row>
     <row r="6155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6155" t="s">
-        <v>6183</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="6156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6156" t="s">
         <v>6184</v>
+      </c>
+    </row>
+    <row r="6157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6157" t="s">
+        <v>6185</v>
       </c>
     </row>
   </sheetData>
@@ -68259,19 +68270,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6185</v>
+        <v>6186</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6186</v>
+        <v>6187</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68282,13 +68293,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68299,13 +68310,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68316,13 +68327,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68333,13 +68344,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68350,13 +68361,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68367,13 +68378,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68384,13 +68395,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68401,13 +68412,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68418,13 +68429,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68435,13 +68446,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68452,13 +68463,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68469,13 +68480,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68486,13 +68497,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68503,13 +68514,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68520,13 +68531,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 29/09/2025
Atualização de arquivo: 29/09/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F18A6D-0E1E-483E-9937-A29149E7190C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354945A5-95A8-4F1E-874A-AC3D2D20809F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6239" uniqueCount="6194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6242" uniqueCount="6197">
   <si>
     <t>Fecha</t>
   </si>
@@ -18570,10 +18570,19 @@
     <t>2025/09/25</t>
   </si>
   <si>
+    <t>2025/09/26</t>
+  </si>
+  <si>
+    <t>2025/09/27</t>
+  </si>
+  <si>
+    <t>2025/09/28</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República viernes, 26 de septiembre de 2025 7:31:53 a. m.</t>
+    <t>Descargado de sistema del Banco de la República lunes, 29 de septiembre de 2025 7:57:26 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -18989,10 +18998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6157"/>
+  <dimension ref="A1:B6160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68236,15 +68245,39 @@
       <c r="A6155" t="s">
         <v>6184</v>
       </c>
+      <c r="B6155" s="1">
+        <v>4558.5587999999998</v>
+      </c>
     </row>
     <row r="6156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6156" t="s">
-        <v>6184</v>
+        <v>6185</v>
+      </c>
+      <c r="B6156" s="1">
+        <v>4569.3738999999996</v>
       </c>
     </row>
     <row r="6157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6157" t="s">
-        <v>6185</v>
+        <v>6186</v>
+      </c>
+      <c r="B6157" s="1">
+        <v>4569.3738999999996</v>
+      </c>
+    </row>
+    <row r="6158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6158" t="s">
+        <v>6187</v>
+      </c>
+    </row>
+    <row r="6159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6159" t="s">
+        <v>6187</v>
+      </c>
+    </row>
+    <row r="6160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6160" t="s">
+        <v>6188</v>
       </c>
     </row>
   </sheetData>
@@ -68270,19 +68303,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6186</v>
+        <v>6189</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6187</v>
+        <v>6190</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6188</v>
+        <v>6191</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6189</v>
+        <v>6192</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6190</v>
+        <v>6193</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68293,13 +68326,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68310,13 +68343,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68327,13 +68360,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68344,13 +68377,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68361,13 +68394,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68378,13 +68411,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68395,13 +68428,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68412,13 +68445,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68429,13 +68462,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68446,13 +68479,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68463,13 +68496,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68480,13 +68513,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68497,13 +68530,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68514,13 +68547,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68531,13 +68564,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6191</v>
+        <v>6194</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6192</v>
+        <v>6195</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 01/10/2025
Atualização de arquivo: 01/10/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354945A5-95A8-4F1E-874A-AC3D2D20809F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C1AD25-175F-4481-B8BC-1BA7C898D388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6242" uniqueCount="6197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6244" uniqueCount="6199">
   <si>
     <t>Fecha</t>
   </si>
@@ -18579,10 +18579,16 @@
     <t>2025/09/28</t>
   </si>
   <si>
+    <t>2025/09/29</t>
+  </si>
+  <si>
+    <t>2025/09/30</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República lunes, 29 de septiembre de 2025 7:57:26 a. m.</t>
+    <t>Descargado de sistema del Banco de la República miércoles, 1 de octubre de 2025 8:10:26 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -18998,10 +19004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6160"/>
+  <dimension ref="A1:B6162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68269,15 +68275,31 @@
       <c r="A6158" t="s">
         <v>6187</v>
       </c>
+      <c r="B6158" s="1">
+        <v>4584.2247600000001</v>
+      </c>
     </row>
     <row r="6159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6159" t="s">
-        <v>6187</v>
+        <v>6188</v>
+      </c>
+      <c r="B6159" s="1">
+        <v>4584.0157499999996</v>
       </c>
     </row>
     <row r="6160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6160" t="s">
-        <v>6188</v>
+        <v>6189</v>
+      </c>
+    </row>
+    <row r="6161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6161" t="s">
+        <v>6189</v>
+      </c>
+    </row>
+    <row r="6162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6162" t="s">
+        <v>6190</v>
       </c>
     </row>
   </sheetData>
@@ -68303,19 +68325,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6189</v>
+        <v>6191</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6190</v>
+        <v>6192</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6191</v>
+        <v>6193</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6192</v>
+        <v>6194</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6193</v>
+        <v>6195</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68326,13 +68348,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68343,13 +68365,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68360,13 +68382,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68377,13 +68399,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68394,13 +68416,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68411,13 +68433,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68428,13 +68450,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68445,13 +68467,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68462,13 +68484,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68479,13 +68501,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68496,13 +68518,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68513,13 +68535,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68530,13 +68552,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68547,13 +68569,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68564,13 +68586,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 03/10/2025
Atualização de arquivo: 03/10/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C1AD25-175F-4481-B8BC-1BA7C898D388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5033BE-FC57-4E2A-AE36-68698C90F91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6244" uniqueCount="6199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6246" uniqueCount="6201">
   <si>
     <t>Fecha</t>
   </si>
@@ -18585,10 +18585,16 @@
     <t>2025/09/30</t>
   </si>
   <si>
+    <t>2025/10/01</t>
+  </si>
+  <si>
+    <t>2025/10/02</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República miércoles, 1 de octubre de 2025 8:10:26 a. m.</t>
+    <t>Descargado de sistema del Banco de la República viernes, 3 de octubre de 2025 8:08:16 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19004,10 +19010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6162"/>
+  <dimension ref="A1:B6164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68291,15 +68297,31 @@
       <c r="A6160" t="s">
         <v>6189</v>
       </c>
-    </row>
-    <row r="6161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6160" s="1">
+        <v>4608.2094699999998</v>
+      </c>
+    </row>
+    <row r="6161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6161" t="s">
-        <v>6189</v>
-      </c>
-    </row>
-    <row r="6162" spans="1:1" x14ac:dyDescent="0.3">
+        <v>6190</v>
+      </c>
+      <c r="B6161" s="1">
+        <v>4556.5514999999996</v>
+      </c>
+    </row>
+    <row r="6162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6162" t="s">
-        <v>6190</v>
+        <v>6191</v>
+      </c>
+    </row>
+    <row r="6163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6163" t="s">
+        <v>6191</v>
+      </c>
+    </row>
+    <row r="6164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6164" t="s">
+        <v>6192</v>
       </c>
     </row>
   </sheetData>
@@ -68325,19 +68347,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6191</v>
+        <v>6193</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6192</v>
+        <v>6194</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6193</v>
+        <v>6195</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6194</v>
+        <v>6196</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6195</v>
+        <v>6197</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68348,13 +68370,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68365,13 +68387,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68382,13 +68404,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68399,13 +68421,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68416,13 +68438,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68433,13 +68455,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68450,13 +68472,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68467,13 +68489,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68484,13 +68506,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68501,13 +68523,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68518,13 +68540,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68535,13 +68557,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68552,13 +68574,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68569,13 +68591,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68586,13 +68608,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6196</v>
+        <v>6198</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6197</v>
+        <v>6199</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6198</v>
+        <v>6200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 06/10/2025
Atualização de arquivo: 06/10/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5033BE-FC57-4E2A-AE36-68698C90F91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52AA5F7-E602-4918-9667-72E4A3B53293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6246" uniqueCount="6201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6249" uniqueCount="6204">
   <si>
     <t>Fecha</t>
   </si>
@@ -18591,10 +18591,19 @@
     <t>2025/10/02</t>
   </si>
   <si>
+    <t>2025/10/03</t>
+  </si>
+  <si>
+    <t>2025/10/04</t>
+  </si>
+  <si>
+    <t>2025/10/05</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República viernes, 3 de octubre de 2025 8:08:16 a. m.</t>
+    <t>Descargado de sistema del Banco de la República lunes, 6 de octubre de 2025 9:30:38 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19010,10 +19019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6164"/>
+  <dimension ref="A1:B6167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68313,15 +68322,39 @@
       <c r="A6162" t="s">
         <v>6191</v>
       </c>
+      <c r="B6162" s="1">
+        <v>4576.0242399999997</v>
+      </c>
     </row>
     <row r="6163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6163" t="s">
-        <v>6191</v>
+        <v>6192</v>
+      </c>
+      <c r="B6163" s="1">
+        <v>4548.4810200000002</v>
       </c>
     </row>
     <row r="6164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6164" t="s">
-        <v>6192</v>
+        <v>6193</v>
+      </c>
+      <c r="B6164" s="1">
+        <v>4548.4810200000002</v>
+      </c>
+    </row>
+    <row r="6165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6165" t="s">
+        <v>6194</v>
+      </c>
+    </row>
+    <row r="6166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6166" t="s">
+        <v>6194</v>
+      </c>
+    </row>
+    <row r="6167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6167" t="s">
+        <v>6195</v>
       </c>
     </row>
   </sheetData>
@@ -68347,19 +68380,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6193</v>
+        <v>6196</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6194</v>
+        <v>6197</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6195</v>
+        <v>6198</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6196</v>
+        <v>6199</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6197</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68370,13 +68403,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68387,13 +68420,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68404,13 +68437,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68421,13 +68454,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68438,13 +68471,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68455,13 +68488,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68472,13 +68505,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68489,13 +68522,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68506,13 +68539,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68523,13 +68556,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68540,13 +68573,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68557,13 +68590,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68574,13 +68607,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68591,13 +68624,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68608,13 +68641,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 09/10/2025
Atualização de arquivo: 09/10/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52AA5F7-E602-4918-9667-72E4A3B53293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AF587E-73D2-4938-98C1-5665AE572201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6249" uniqueCount="6204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6252" uniqueCount="6207">
   <si>
     <t>Fecha</t>
   </si>
@@ -18600,10 +18600,19 @@
     <t>2025/10/05</t>
   </si>
   <si>
+    <t>2025/10/06</t>
+  </si>
+  <si>
+    <t>2025/10/07</t>
+  </si>
+  <si>
+    <t>2025/10/08</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República lunes, 6 de octubre de 2025 9:30:38 a. m.</t>
+    <t>Descargado de sistema del Banco de la República jueves, 9 de octubre de 2025 8:02:21 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19019,10 +19028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6167"/>
+  <dimension ref="A1:B6170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68346,15 +68355,39 @@
       <c r="A6165" t="s">
         <v>6194</v>
       </c>
+      <c r="B6165" s="1">
+        <v>4539.1829900000002</v>
+      </c>
     </row>
     <row r="6166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6166" t="s">
-        <v>6194</v>
+        <v>6195</v>
+      </c>
+      <c r="B6166" s="1">
+        <v>4494.3608100000001</v>
       </c>
     </row>
     <row r="6167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6167" t="s">
-        <v>6195</v>
+        <v>6196</v>
+      </c>
+      <c r="B6167" s="1">
+        <v>4494.4682300000004</v>
+      </c>
+    </row>
+    <row r="6168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6168" t="s">
+        <v>6197</v>
+      </c>
+    </row>
+    <row r="6169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6169" t="s">
+        <v>6197</v>
+      </c>
+    </row>
+    <row r="6170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6170" t="s">
+        <v>6198</v>
       </c>
     </row>
   </sheetData>
@@ -68380,19 +68413,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6196</v>
+        <v>6199</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6197</v>
+        <v>6200</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6198</v>
+        <v>6201</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6199</v>
+        <v>6202</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6200</v>
+        <v>6203</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68403,13 +68436,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68420,13 +68453,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68437,13 +68470,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68454,13 +68487,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68471,13 +68504,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68488,13 +68521,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68505,13 +68538,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68522,13 +68555,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68539,13 +68572,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68556,13 +68589,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68573,13 +68606,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68590,13 +68623,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68607,13 +68640,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68624,13 +68657,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68641,13 +68674,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6201</v>
+        <v>6204</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6202</v>
+        <v>6205</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6203</v>
+        <v>6206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 13/10/2025
Atualização de arquivo: 13/10/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AF587E-73D2-4938-98C1-5665AE572201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9487EE-6DB3-42AF-9FA3-2A9CD5F6CB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6252" uniqueCount="6207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6256" uniqueCount="6211">
   <si>
     <t>Fecha</t>
   </si>
@@ -18609,10 +18609,22 @@
     <t>2025/10/08</t>
   </si>
   <si>
+    <t>2025/10/09</t>
+  </si>
+  <si>
+    <t>2025/10/10</t>
+  </si>
+  <si>
+    <t>2025/10/11</t>
+  </si>
+  <si>
+    <t>2025/10/12</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República jueves, 9 de octubre de 2025 8:02:21 a. m.</t>
+    <t>Descargado de sistema del Banco de la República lunes, 13 de octubre de 2025 9:02:00 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19028,10 +19040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6170"/>
+  <dimension ref="A1:B6174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68379,15 +68391,47 @@
       <c r="A6168" t="s">
         <v>6197</v>
       </c>
+      <c r="B6168" s="1">
+        <v>4493.3903700000001</v>
+      </c>
     </row>
     <row r="6169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6169" t="s">
-        <v>6197</v>
+        <v>6198</v>
+      </c>
+      <c r="B6169" s="1">
+        <v>4510.3984200000004</v>
       </c>
     </row>
     <row r="6170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6170" t="s">
-        <v>6198</v>
+        <v>6199</v>
+      </c>
+      <c r="B6170" s="1">
+        <v>4531.5319200000004</v>
+      </c>
+    </row>
+    <row r="6171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6171" t="s">
+        <v>6200</v>
+      </c>
+      <c r="B6171" s="1">
+        <v>4531.5319200000004</v>
+      </c>
+    </row>
+    <row r="6172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6172" t="s">
+        <v>6201</v>
+      </c>
+    </row>
+    <row r="6173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6173" t="s">
+        <v>6201</v>
+      </c>
+    </row>
+    <row r="6174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6174" t="s">
+        <v>6202</v>
       </c>
     </row>
   </sheetData>
@@ -68413,19 +68457,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6199</v>
+        <v>6203</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6200</v>
+        <v>6204</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6201</v>
+        <v>6205</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6202</v>
+        <v>6206</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6203</v>
+        <v>6207</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68436,13 +68480,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68453,13 +68497,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68470,13 +68514,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68487,13 +68531,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68504,13 +68548,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68521,13 +68565,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68538,13 +68582,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68555,13 +68599,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68572,13 +68616,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68589,13 +68633,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68606,13 +68650,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68623,13 +68667,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68640,13 +68684,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68657,13 +68701,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68674,13 +68718,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6204</v>
+        <v>6208</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6205</v>
+        <v>6209</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6206</v>
+        <v>6210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 14/10/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9487EE-6DB3-42AF-9FA3-2A9CD5F6CB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29066E4A-66A7-410F-B1EA-DD9B06D8333E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6256" uniqueCount="6211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6257" uniqueCount="6212">
   <si>
     <t>Fecha</t>
   </si>
@@ -18621,10 +18621,13 @@
     <t>2025/10/12</t>
   </si>
   <si>
+    <t>2025/10/13</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República lunes, 13 de octubre de 2025 9:02:00 a. m.</t>
+    <t>Descargado de sistema del Banco de la República martes, 14 de octubre de 2025 8:20:22 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19040,10 +19043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6174"/>
+  <dimension ref="A1:B6175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68423,15 +68426,23 @@
       <c r="A6172" t="s">
         <v>6201</v>
       </c>
+      <c r="B6172" s="1">
+        <v>4524.0967600000004</v>
+      </c>
     </row>
     <row r="6173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6173" t="s">
-        <v>6201</v>
+        <v>6202</v>
       </c>
     </row>
     <row r="6174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6174" t="s">
         <v>6202</v>
+      </c>
+    </row>
+    <row r="6175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6175" t="s">
+        <v>6203</v>
       </c>
     </row>
   </sheetData>
@@ -68457,19 +68468,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6203</v>
+        <v>6204</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6204</v>
+        <v>6205</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6205</v>
+        <v>6206</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6206</v>
+        <v>6207</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6207</v>
+        <v>6208</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68480,13 +68491,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68497,13 +68508,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68514,13 +68525,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68531,13 +68542,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68548,13 +68559,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68565,13 +68576,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68582,13 +68593,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68599,13 +68610,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68616,13 +68627,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68633,13 +68644,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68650,13 +68661,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68667,13 +68678,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68684,13 +68695,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68701,13 +68712,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68718,13 +68729,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 17/10/2025
Atualização de arquivo: 17/10/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29066E4A-66A7-410F-B1EA-DD9B06D8333E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B19F5B-0775-4DC5-9319-D540EE7E8EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6257" uniqueCount="6212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6260" uniqueCount="6215">
   <si>
     <t>Fecha</t>
   </si>
@@ -18624,10 +18624,19 @@
     <t>2025/10/13</t>
   </si>
   <si>
+    <t>2025/10/14</t>
+  </si>
+  <si>
+    <t>2025/10/15</t>
+  </si>
+  <si>
+    <t>2025/10/16</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República martes, 14 de octubre de 2025 8:20:22 a. m.</t>
+    <t>Descargado de sistema del Banco de la República viernes, 17 de octubre de 2025 9:53:01 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19043,10 +19052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6175"/>
+  <dimension ref="A1:B6178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68434,15 +68443,39 @@
       <c r="A6173" t="s">
         <v>6202</v>
       </c>
+      <c r="B6173" s="1">
+        <v>4537.2061100000001</v>
+      </c>
     </row>
     <row r="6174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6174" t="s">
-        <v>6202</v>
+        <v>6203</v>
+      </c>
+      <c r="B6174" s="1">
+        <v>4572.0795399999997</v>
       </c>
     </row>
     <row r="6175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6175" t="s">
-        <v>6203</v>
+        <v>6204</v>
+      </c>
+      <c r="B6175" s="1">
+        <v>4556.5522300000002</v>
+      </c>
+    </row>
+    <row r="6176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6176" t="s">
+        <v>6205</v>
+      </c>
+    </row>
+    <row r="6177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6177" t="s">
+        <v>6205</v>
+      </c>
+    </row>
+    <row r="6178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6178" t="s">
+        <v>6206</v>
       </c>
     </row>
   </sheetData>
@@ -68468,19 +68501,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6204</v>
+        <v>6207</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6205</v>
+        <v>6208</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6206</v>
+        <v>6209</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6207</v>
+        <v>6210</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6208</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68491,13 +68524,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68508,13 +68541,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68525,13 +68558,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68542,13 +68575,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68559,13 +68592,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68576,13 +68609,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68593,13 +68626,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68610,13 +68643,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68627,13 +68660,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68644,13 +68677,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68661,13 +68694,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68678,13 +68711,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68695,13 +68728,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68712,13 +68745,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68729,13 +68762,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6209</v>
+        <v>6212</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6210</v>
+        <v>6213</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6211</v>
+        <v>6214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 21/10/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B19F5B-0775-4DC5-9319-D540EE7E8EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5D03E3-7C89-4786-92F2-74B0D233C692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6260" uniqueCount="6215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6264" uniqueCount="6219">
   <si>
     <t>Fecha</t>
   </si>
@@ -18633,10 +18633,22 @@
     <t>2025/10/16</t>
   </si>
   <si>
+    <t>2025/10/17</t>
+  </si>
+  <si>
+    <t>2025/10/18</t>
+  </si>
+  <si>
+    <t>2025/10/19</t>
+  </si>
+  <si>
+    <t>2025/10/20</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República viernes, 17 de octubre de 2025 9:53:01 a. m.</t>
+    <t>Descargado de sistema del Banco de la República martes, 21 de octubre de 2025 7:58:19 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19052,10 +19064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6178"/>
+  <dimension ref="A1:B6182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68467,15 +68479,47 @@
       <c r="A6176" t="s">
         <v>6205</v>
       </c>
-    </row>
-    <row r="6177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6176" s="1">
+        <v>4523.5714200000002</v>
+      </c>
+    </row>
+    <row r="6177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6177" t="s">
-        <v>6205</v>
-      </c>
-    </row>
-    <row r="6178" spans="1:1" x14ac:dyDescent="0.3">
+        <v>6206</v>
+      </c>
+      <c r="B6177" s="1">
+        <v>4443.1240100000005</v>
+      </c>
+    </row>
+    <row r="6178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6178" t="s">
-        <v>6206</v>
+        <v>6207</v>
+      </c>
+      <c r="B6178" s="1">
+        <v>4443.1240100000005</v>
+      </c>
+    </row>
+    <row r="6179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6179" t="s">
+        <v>6208</v>
+      </c>
+      <c r="B6179" s="1">
+        <v>4437.9830400000001</v>
+      </c>
+    </row>
+    <row r="6180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6180" t="s">
+        <v>6209</v>
+      </c>
+    </row>
+    <row r="6181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6181" t="s">
+        <v>6209</v>
+      </c>
+    </row>
+    <row r="6182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6182" t="s">
+        <v>6210</v>
       </c>
     </row>
   </sheetData>
@@ -68501,19 +68545,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6207</v>
+        <v>6211</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6208</v>
+        <v>6212</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6209</v>
+        <v>6213</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6210</v>
+        <v>6214</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6211</v>
+        <v>6215</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68524,13 +68568,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68541,13 +68585,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68558,13 +68602,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68575,13 +68619,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68592,13 +68636,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68609,13 +68653,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68626,13 +68670,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68643,13 +68687,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68660,13 +68704,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68677,13 +68721,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68694,13 +68738,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68711,13 +68755,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68728,13 +68772,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68745,13 +68789,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68762,13 +68806,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6212</v>
+        <v>6216</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6213</v>
+        <v>6217</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6214</v>
+        <v>6218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 23/10/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5D03E3-7C89-4786-92F2-74B0D233C692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E15819-01FD-4C91-A956-67BD535899D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6264" uniqueCount="6219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6266" uniqueCount="6221">
   <si>
     <t>Fecha</t>
   </si>
@@ -18645,10 +18645,16 @@
     <t>2025/10/20</t>
   </si>
   <si>
+    <t>2025/10/21</t>
+  </si>
+  <si>
+    <t>2025/10/22</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República martes, 21 de octubre de 2025 7:58:19 a. m.</t>
+    <t>Descargado de sistema del Banco de la República jueves, 23 de octubre de 2025 7:28:10 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19064,10 +19070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6182"/>
+  <dimension ref="A1:B6184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68511,15 +68517,31 @@
       <c r="A6180" t="s">
         <v>6209</v>
       </c>
+      <c r="B6180" s="1">
+        <v>4499.36636</v>
+      </c>
     </row>
     <row r="6181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6181" t="s">
-        <v>6209</v>
+        <v>6210</v>
+      </c>
+      <c r="B6181" s="1">
+        <v>4501.3140899999999</v>
       </c>
     </row>
     <row r="6182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6182" t="s">
-        <v>6210</v>
+        <v>6211</v>
+      </c>
+    </row>
+    <row r="6183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6183" t="s">
+        <v>6211</v>
+      </c>
+    </row>
+    <row r="6184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6184" t="s">
+        <v>6212</v>
       </c>
     </row>
   </sheetData>
@@ -68545,19 +68567,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6211</v>
+        <v>6213</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6212</v>
+        <v>6214</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6213</v>
+        <v>6215</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6214</v>
+        <v>6216</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6215</v>
+        <v>6217</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68568,13 +68590,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68585,13 +68607,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68602,13 +68624,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68619,13 +68641,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68636,13 +68658,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68653,13 +68675,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68670,13 +68692,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68687,13 +68709,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68704,13 +68726,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68721,13 +68743,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68738,13 +68760,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68755,13 +68777,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68772,13 +68794,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68789,13 +68811,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68806,13 +68828,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6216</v>
+        <v>6218</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6217</v>
+        <v>6219</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 28/10/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E15819-01FD-4C91-A956-67BD535899D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53D2DCC-AE84-4436-A0BC-31017DDE5D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6266" uniqueCount="6221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6271" uniqueCount="6226">
   <si>
     <t>Fecha</t>
   </si>
@@ -18651,10 +18651,25 @@
     <t>2025/10/22</t>
   </si>
   <si>
+    <t>2025/10/23</t>
+  </si>
+  <si>
+    <t>2025/10/24</t>
+  </si>
+  <si>
+    <t>2025/10/25</t>
+  </si>
+  <si>
+    <t>2025/10/26</t>
+  </si>
+  <si>
+    <t>2025/10/27</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República jueves, 23 de octubre de 2025 7:28:10 a. m.</t>
+    <t>Descargado de sistema del Banco de la República martes, 28 de octubre de 2025 7:41:27 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19070,10 +19085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6184"/>
+  <dimension ref="A1:B6189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I7" sqref="H7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68533,15 +68548,55 @@
       <c r="A6182" t="s">
         <v>6211</v>
       </c>
+      <c r="B6182" s="1">
+        <v>4530.4123399999999</v>
+      </c>
     </row>
     <row r="6183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6183" t="s">
-        <v>6211</v>
+        <v>6212</v>
+      </c>
+      <c r="B6183" s="1">
+        <v>4521.0723699999999</v>
       </c>
     </row>
     <row r="6184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6184" t="s">
-        <v>6212</v>
+        <v>6213</v>
+      </c>
+      <c r="B6184" s="1">
+        <v>4486.0432300000002</v>
+      </c>
+    </row>
+    <row r="6185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6185" t="s">
+        <v>6214</v>
+      </c>
+      <c r="B6185" s="1">
+        <v>4486.0432300000002</v>
+      </c>
+    </row>
+    <row r="6186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6186" t="s">
+        <v>6215</v>
+      </c>
+      <c r="B6186" s="1">
+        <v>4489.7089299999998</v>
+      </c>
+    </row>
+    <row r="6187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6187" t="s">
+        <v>6216</v>
+      </c>
+    </row>
+    <row r="6188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6188" t="s">
+        <v>6216</v>
+      </c>
+    </row>
+    <row r="6189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6189" t="s">
+        <v>6217</v>
       </c>
     </row>
   </sheetData>
@@ -68567,19 +68622,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6213</v>
+        <v>6218</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6214</v>
+        <v>6219</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6215</v>
+        <v>6220</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6216</v>
+        <v>6221</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6217</v>
+        <v>6222</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68590,13 +68645,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68607,13 +68662,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68624,13 +68679,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68641,13 +68696,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68658,13 +68713,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68675,13 +68730,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68692,13 +68747,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68709,13 +68764,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68726,13 +68781,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68743,13 +68798,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68760,13 +68815,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68777,13 +68832,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68794,13 +68849,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68811,13 +68866,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68828,13 +68883,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6218</v>
+        <v>6223</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6219</v>
+        <v>6224</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6220</v>
+        <v>6225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 30/10/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53D2DCC-AE84-4436-A0BC-31017DDE5D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD313B68-C435-4D4E-954F-273D45B717A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6271" uniqueCount="6226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6273" uniqueCount="6228">
   <si>
     <t>Fecha</t>
   </si>
@@ -18666,10 +18666,16 @@
     <t>2025/10/27</t>
   </si>
   <si>
+    <t>2025/10/28</t>
+  </si>
+  <si>
+    <t>2025/10/29</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República martes, 28 de octubre de 2025 7:41:27 a. m.</t>
+    <t>Descargado de sistema del Banco de la República jueves, 30 de octubre de 2025 7:53:29 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19085,10 +19091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6189"/>
+  <dimension ref="A1:B6191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="H7:I7"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68588,15 +68594,31 @@
       <c r="A6187" t="s">
         <v>6216</v>
       </c>
+      <c r="B6187" s="1">
+        <v>4481.7605700000004</v>
+      </c>
     </row>
     <row r="6188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6188" t="s">
-        <v>6216</v>
+        <v>6217</v>
+      </c>
+      <c r="B6188" s="1">
+        <v>4519.61337</v>
       </c>
     </row>
     <row r="6189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6189" t="s">
-        <v>6217</v>
+        <v>6218</v>
+      </c>
+    </row>
+    <row r="6190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6190" t="s">
+        <v>6218</v>
+      </c>
+    </row>
+    <row r="6191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6191" t="s">
+        <v>6219</v>
       </c>
     </row>
   </sheetData>
@@ -68622,19 +68644,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6218</v>
+        <v>6220</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6219</v>
+        <v>6221</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6220</v>
+        <v>6222</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6221</v>
+        <v>6223</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6222</v>
+        <v>6224</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68645,13 +68667,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68662,13 +68684,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68679,13 +68701,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68696,13 +68718,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68713,13 +68735,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68730,13 +68752,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68747,13 +68769,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68764,13 +68786,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68781,13 +68803,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68798,13 +68820,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68815,13 +68837,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68832,13 +68854,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68849,13 +68871,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68866,13 +68888,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68883,13 +68905,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6223</v>
+        <v>6225</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6224</v>
+        <v>6226</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6225</v>
+        <v>6227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 03/11/2025
Atualização de arquivo: 03/11/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD313B68-C435-4D4E-954F-273D45B717A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CB6093-5F07-4503-A828-93D690F7902B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6273" uniqueCount="6228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6277" uniqueCount="6232">
   <si>
     <t>Fecha</t>
   </si>
@@ -18672,10 +18672,22 @@
     <t>2025/10/29</t>
   </si>
   <si>
+    <t>2025/10/30</t>
+  </si>
+  <si>
+    <t>2025/10/31</t>
+  </si>
+  <si>
+    <t>2025/11/01</t>
+  </si>
+  <si>
+    <t>2025/11/02</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República jueves, 30 de octubre de 2025 7:53:29 a. m.</t>
+    <t>Descargado de sistema del Banco de la República lunes, 3 de noviembre de 2025 8:31:39 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19091,10 +19103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6191"/>
+  <dimension ref="A1:B6195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68610,15 +68622,47 @@
       <c r="A6189" t="s">
         <v>6218</v>
       </c>
+      <c r="B6189" s="1">
+        <v>4492.9493499999999</v>
+      </c>
     </row>
     <row r="6190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6190" t="s">
-        <v>6218</v>
+        <v>6219</v>
+      </c>
+      <c r="B6190" s="1">
+        <v>4467.2387600000002</v>
       </c>
     </row>
     <row r="6191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6191" t="s">
-        <v>6219</v>
+        <v>6220</v>
+      </c>
+      <c r="B6191" s="1">
+        <v>4455.3504999999996</v>
+      </c>
+    </row>
+    <row r="6192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6192" t="s">
+        <v>6221</v>
+      </c>
+      <c r="B6192" s="1">
+        <v>4455.3504999999996</v>
+      </c>
+    </row>
+    <row r="6193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6193" t="s">
+        <v>6222</v>
+      </c>
+    </row>
+    <row r="6194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6194" t="s">
+        <v>6222</v>
+      </c>
+    </row>
+    <row r="6195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6195" t="s">
+        <v>6223</v>
       </c>
     </row>
   </sheetData>
@@ -68644,19 +68688,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6220</v>
+        <v>6224</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6221</v>
+        <v>6225</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6222</v>
+        <v>6226</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6223</v>
+        <v>6227</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6224</v>
+        <v>6228</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68667,13 +68711,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68684,13 +68728,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68701,13 +68745,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68718,13 +68762,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68735,13 +68779,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68752,13 +68796,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68769,13 +68813,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68786,13 +68830,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68803,13 +68847,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68820,13 +68864,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68837,13 +68881,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68854,13 +68898,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68871,13 +68915,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68888,13 +68932,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68905,13 +68949,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6225</v>
+        <v>6229</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6226</v>
+        <v>6230</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 06/11/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CB6093-5F07-4503-A828-93D690F7902B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF20F0E-5E0D-4981-8B63-AE8A2C15C291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6277" uniqueCount="6232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6280" uniqueCount="6235">
   <si>
     <t>Fecha</t>
   </si>
@@ -18684,10 +18684,19 @@
     <t>2025/11/02</t>
   </si>
   <si>
+    <t>2025/11/03</t>
+  </si>
+  <si>
+    <t>2025/11/04</t>
+  </si>
+  <si>
+    <t>2025/11/05</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República lunes, 3 de noviembre de 2025 8:31:39 a. m.</t>
+    <t>Descargado de sistema del Banco de la República jueves, 6 de noviembre de 2025 8:01:21 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19103,10 +19112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6195"/>
+  <dimension ref="A1:B6198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68650,19 +68659,43 @@
         <v>4455.3504999999996</v>
       </c>
     </row>
-    <row r="6193" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6193" t="s">
         <v>6222</v>
       </c>
-    </row>
-    <row r="6194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6193" s="1">
+        <v>4448.5952900000002</v>
+      </c>
+    </row>
+    <row r="6194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6194" t="s">
-        <v>6222</v>
-      </c>
-    </row>
-    <row r="6195" spans="1:1" x14ac:dyDescent="0.3">
+        <v>6223</v>
+      </c>
+      <c r="B6194" s="1">
+        <v>4436.0499</v>
+      </c>
+    </row>
+    <row r="6195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6195" t="s">
-        <v>6223</v>
+        <v>6224</v>
+      </c>
+      <c r="B6195" s="1">
+        <v>4445.20831</v>
+      </c>
+    </row>
+    <row r="6196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6196" t="s">
+        <v>6225</v>
+      </c>
+    </row>
+    <row r="6197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6197" t="s">
+        <v>6225</v>
+      </c>
+    </row>
+    <row r="6198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6198" t="s">
+        <v>6226</v>
       </c>
     </row>
   </sheetData>
@@ -68688,19 +68721,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6224</v>
+        <v>6227</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6225</v>
+        <v>6228</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6226</v>
+        <v>6229</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6227</v>
+        <v>6230</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6228</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68711,13 +68744,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68728,13 +68761,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68745,13 +68778,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68762,13 +68795,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68779,13 +68812,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68796,13 +68829,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68813,13 +68846,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68830,13 +68863,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68847,13 +68880,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68864,13 +68897,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68881,13 +68914,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68898,13 +68931,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68915,13 +68948,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68932,13 +68965,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68949,13 +68982,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6229</v>
+        <v>6232</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6230</v>
+        <v>6233</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 10/11/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF20F0E-5E0D-4981-8B63-AE8A2C15C291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA46D24-FDA1-4904-822B-C211FD2CCA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6280" uniqueCount="6235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6284" uniqueCount="6239">
   <si>
     <t>Fecha</t>
   </si>
@@ -18693,10 +18693,22 @@
     <t>2025/11/05</t>
   </si>
   <si>
+    <t>2025/11/06</t>
+  </si>
+  <si>
+    <t>2025/11/07</t>
+  </si>
+  <si>
+    <t>2025/11/08</t>
+  </si>
+  <si>
+    <t>2025/11/09</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República jueves, 6 de noviembre de 2025 8:01:21 a. m.</t>
+    <t>Descargado de sistema del Banco de la República lunes, 10 de noviembre de 2025 8:25:00 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19112,10 +19124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6198"/>
+  <dimension ref="A1:B6202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68687,15 +68699,47 @@
       <c r="A6196" t="s">
         <v>6225</v>
       </c>
+      <c r="B6196" s="1">
+        <v>4430.5564000000004</v>
+      </c>
     </row>
     <row r="6197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6197" t="s">
-        <v>6225</v>
+        <v>6226</v>
+      </c>
+      <c r="B6197" s="1">
+        <v>4405.7201800000003</v>
       </c>
     </row>
     <row r="6198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6198" t="s">
-        <v>6226</v>
+        <v>6227</v>
+      </c>
+      <c r="B6198" s="1">
+        <v>4373.4791999999998</v>
+      </c>
+    </row>
+    <row r="6199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6199" t="s">
+        <v>6228</v>
+      </c>
+      <c r="B6199" s="1">
+        <v>4373.4791999999998</v>
+      </c>
+    </row>
+    <row r="6200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6200" t="s">
+        <v>6229</v>
+      </c>
+    </row>
+    <row r="6201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6201" t="s">
+        <v>6229</v>
+      </c>
+    </row>
+    <row r="6202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6202" t="s">
+        <v>6230</v>
       </c>
     </row>
   </sheetData>
@@ -68721,19 +68765,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6227</v>
+        <v>6231</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6228</v>
+        <v>6232</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6229</v>
+        <v>6233</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6230</v>
+        <v>6234</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6231</v>
+        <v>6235</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68744,13 +68788,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68761,13 +68805,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68778,13 +68822,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68795,13 +68839,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68812,13 +68856,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68829,13 +68873,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68846,13 +68890,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68863,13 +68907,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68880,13 +68924,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68897,13 +68941,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68914,13 +68958,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68931,13 +68975,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68948,13 +68992,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68965,13 +69009,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68982,13 +69026,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6232</v>
+        <v>6236</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6233</v>
+        <v>6237</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de arquivo: 13/11/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA46D24-FDA1-4904-822B-C211FD2CCA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC7EE7B-7FBA-4655-AFF0-499AD38F2D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6284" uniqueCount="6239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6287" uniqueCount="6242">
   <si>
     <t>Fecha</t>
   </si>
@@ -18705,10 +18705,19 @@
     <t>2025/11/09</t>
   </si>
   <si>
+    <t>2025/11/10</t>
+  </si>
+  <si>
+    <t>2025/11/11</t>
+  </si>
+  <si>
+    <t>2025/11/12</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República lunes, 10 de noviembre de 2025 8:25:00 a. m.</t>
+    <t>Descargado de sistema del Banco de la República jueves, 13 de noviembre de 2025 8:01:51 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19124,10 +19133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6202"/>
+  <dimension ref="A1:B6205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68731,15 +68740,39 @@
       <c r="A6200" t="s">
         <v>6229</v>
       </c>
+      <c r="B6200" s="1">
+        <v>4363.6532800000004</v>
+      </c>
     </row>
     <row r="6201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6201" t="s">
-        <v>6229</v>
+        <v>6230</v>
+      </c>
+      <c r="B6201" s="1">
+        <v>4360.7983299999996</v>
       </c>
     </row>
     <row r="6202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6202" t="s">
-        <v>6230</v>
+        <v>6231</v>
+      </c>
+      <c r="B6202" s="1">
+        <v>4360.7983299999996</v>
+      </c>
+    </row>
+    <row r="6203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6203" t="s">
+        <v>6232</v>
+      </c>
+    </row>
+    <row r="6204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6204" t="s">
+        <v>6232</v>
+      </c>
+    </row>
+    <row r="6205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6205" t="s">
+        <v>6233</v>
       </c>
     </row>
   </sheetData>
@@ -68765,19 +68798,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6231</v>
+        <v>6234</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6232</v>
+        <v>6235</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6233</v>
+        <v>6236</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6234</v>
+        <v>6237</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6235</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68788,13 +68821,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68805,13 +68838,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68822,13 +68855,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68839,13 +68872,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68856,13 +68889,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68873,13 +68906,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68890,13 +68923,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68907,13 +68940,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68924,13 +68957,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68941,13 +68974,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68958,13 +68991,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68975,13 +69008,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68992,13 +69025,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69009,13 +69042,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69026,13 +69059,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6236</v>
+        <v>6239</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6237</v>
+        <v>6240</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de dados 17/11/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC7EE7B-7FBA-4655-AFF0-499AD38F2D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6BDA51-B0EB-4597-9718-14290B8C5FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6287" uniqueCount="6242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6291" uniqueCount="6246">
   <si>
     <t>Fecha</t>
   </si>
@@ -18714,10 +18714,22 @@
     <t>2025/11/12</t>
   </si>
   <si>
+    <t>2025/11/13</t>
+  </si>
+  <si>
+    <t>2025/11/14</t>
+  </si>
+  <si>
+    <t>2025/11/15</t>
+  </si>
+  <si>
+    <t>2025/11/16</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República jueves, 13 de noviembre de 2025 8:01:51 a. m.</t>
+    <t>Descargado de sistema del Banco de la República lunes, 17 de noviembre de 2025 8:07:55 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19133,10 +19145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6205"/>
+  <dimension ref="A1:B6209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68764,15 +68776,47 @@
       <c r="A6203" t="s">
         <v>6232</v>
       </c>
+      <c r="B6203" s="1">
+        <v>4329.55645</v>
+      </c>
     </row>
     <row r="6204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6204" t="s">
-        <v>6232</v>
+        <v>6233</v>
+      </c>
+      <c r="B6204" s="1">
+        <v>4319.5714799999996</v>
       </c>
     </row>
     <row r="6205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6205" t="s">
-        <v>6233</v>
+        <v>6234</v>
+      </c>
+      <c r="B6205" s="1">
+        <v>4372.0273999999999</v>
+      </c>
+    </row>
+    <row r="6206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6206" t="s">
+        <v>6235</v>
+      </c>
+      <c r="B6206" s="1">
+        <v>4372.0273999999999</v>
+      </c>
+    </row>
+    <row r="6207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6207" t="s">
+        <v>6236</v>
+      </c>
+    </row>
+    <row r="6208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6208" t="s">
+        <v>6236</v>
+      </c>
+    </row>
+    <row r="6209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6209" t="s">
+        <v>6237</v>
       </c>
     </row>
   </sheetData>
@@ -68798,19 +68842,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6234</v>
+        <v>6238</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6235</v>
+        <v>6239</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6236</v>
+        <v>6240</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6237</v>
+        <v>6241</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6238</v>
+        <v>6242</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68821,13 +68865,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68838,13 +68882,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68855,13 +68899,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68872,13 +68916,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68889,13 +68933,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68906,13 +68950,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68923,13 +68967,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68940,13 +68984,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68957,13 +69001,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68974,13 +69018,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68991,13 +69035,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69008,13 +69052,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69025,13 +69069,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69042,13 +69086,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69059,13 +69103,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6239</v>
+        <v>6243</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6240</v>
+        <v>6244</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de dados 20/11/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6BDA51-B0EB-4597-9718-14290B8C5FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFF3B37-8971-4CBB-9AD8-F534DAA33EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6291" uniqueCount="6246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6294" uniqueCount="6249">
   <si>
     <t>Fecha</t>
   </si>
@@ -18726,10 +18726,19 @@
     <t>2025/11/16</t>
   </si>
   <si>
+    <t>2025/11/17</t>
+  </si>
+  <si>
+    <t>2025/11/18</t>
+  </si>
+  <si>
+    <t>2025/11/19</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República lunes, 17 de noviembre de 2025 8:07:55 a. m.</t>
+    <t>Descargado de sistema del Banco de la República jueves, 20 de noviembre de 2025 9:34:41 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19145,7 +19154,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6209"/>
+  <dimension ref="A1:B6212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -68808,15 +68817,39 @@
       <c r="A6207" t="s">
         <v>6236</v>
       </c>
+      <c r="B6207" s="1">
+        <v>4366.3802400000004</v>
+      </c>
     </row>
     <row r="6208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6208" t="s">
-        <v>6236</v>
-      </c>
-    </row>
-    <row r="6209" spans="1:1" x14ac:dyDescent="0.3">
+        <v>6237</v>
+      </c>
+      <c r="B6208" s="1">
+        <v>4360.3566099999998</v>
+      </c>
+    </row>
+    <row r="6209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6209" t="s">
-        <v>6237</v>
+        <v>6238</v>
+      </c>
+      <c r="B6209" s="1">
+        <v>4315.7489800000003</v>
+      </c>
+    </row>
+    <row r="6210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6210" t="s">
+        <v>6239</v>
+      </c>
+    </row>
+    <row r="6211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6211" t="s">
+        <v>6239</v>
+      </c>
+    </row>
+    <row r="6212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6212" t="s">
+        <v>6240</v>
       </c>
     </row>
   </sheetData>
@@ -68842,19 +68875,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6238</v>
+        <v>6241</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6239</v>
+        <v>6242</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6240</v>
+        <v>6243</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6241</v>
+        <v>6244</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6242</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68865,13 +68898,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68882,13 +68915,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68899,13 +68932,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68916,13 +68949,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68933,13 +68966,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68950,13 +68983,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68967,13 +69000,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68984,13 +69017,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69001,13 +69034,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69018,13 +69051,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69035,13 +69068,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69052,13 +69085,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69069,13 +69102,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69086,13 +69119,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69103,13 +69136,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6243</v>
+        <v>6246</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6244</v>
+        <v>6247</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de dados 24/11/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFF3B37-8971-4CBB-9AD8-F534DAA33EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1504C51-8283-4A92-895A-37CC5B6976FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6294" uniqueCount="6249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6298" uniqueCount="6253">
   <si>
     <t>Fecha</t>
   </si>
@@ -18735,10 +18735,22 @@
     <t>2025/11/19</t>
   </si>
   <si>
+    <t>2025/11/20</t>
+  </si>
+  <si>
+    <t>2025/11/21</t>
+  </si>
+  <si>
+    <t>2025/11/22</t>
+  </si>
+  <si>
+    <t>2025/11/23</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República jueves, 20 de noviembre de 2025 9:34:41 a. m.</t>
+    <t>Descargado de sistema del Banco de la República lunes, 24 de noviembre de 2025 8:01:06 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19154,10 +19166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6212"/>
+  <dimension ref="A1:B6216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68841,15 +68853,47 @@
       <c r="A6210" t="s">
         <v>6239</v>
       </c>
+      <c r="B6210" s="1">
+        <v>4283.9029899999996</v>
+      </c>
     </row>
     <row r="6211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6211" t="s">
-        <v>6239</v>
+        <v>6240</v>
+      </c>
+      <c r="B6211" s="1">
+        <v>4303.0216899999996</v>
       </c>
     </row>
     <row r="6212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6212" t="s">
-        <v>6240</v>
+        <v>6241</v>
+      </c>
+      <c r="B6212" s="1">
+        <v>4380.6568100000004</v>
+      </c>
+    </row>
+    <row r="6213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6213" t="s">
+        <v>6242</v>
+      </c>
+      <c r="B6213" s="1">
+        <v>4380.6568100000004</v>
+      </c>
+    </row>
+    <row r="6214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6214" t="s">
+        <v>6243</v>
+      </c>
+    </row>
+    <row r="6215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6215" t="s">
+        <v>6243</v>
+      </c>
+    </row>
+    <row r="6216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6216" t="s">
+        <v>6244</v>
       </c>
     </row>
   </sheetData>
@@ -68875,19 +68919,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6241</v>
+        <v>6245</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6242</v>
+        <v>6246</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6243</v>
+        <v>6247</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6244</v>
+        <v>6248</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6245</v>
+        <v>6249</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68898,13 +68942,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68915,13 +68959,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68932,13 +68976,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68949,13 +68993,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68966,13 +69010,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68983,13 +69027,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69000,13 +69044,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69017,13 +69061,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69034,13 +69078,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69051,13 +69095,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69068,13 +69112,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69085,13 +69129,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69102,13 +69146,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69119,13 +69163,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69136,13 +69180,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6246</v>
+        <v>6250</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6247</v>
+        <v>6251</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de dados 27/11/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1504C51-8283-4A92-895A-37CC5B6976FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42854D83-0AB9-41EB-A25F-2A38528B3DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6298" uniqueCount="6253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6301" uniqueCount="6256">
   <si>
     <t>Fecha</t>
   </si>
@@ -18747,10 +18747,19 @@
     <t>2025/11/23</t>
   </si>
   <si>
+    <t>2025/11/24</t>
+  </si>
+  <si>
+    <t>2025/11/25</t>
+  </si>
+  <si>
+    <t>2025/11/26</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República lunes, 24 de noviembre de 2025 8:01:06 a. m.</t>
+    <t>Descargado de sistema del Banco de la República jueves, 27 de noviembre de 2025 7:08:35 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19166,10 +19175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6216"/>
+  <dimension ref="A1:B6219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68885,15 +68894,39 @@
       <c r="A6214" t="s">
         <v>6243</v>
       </c>
+      <c r="B6214" s="1">
+        <v>4391.3213699999997</v>
+      </c>
     </row>
     <row r="6215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6215" t="s">
-        <v>6243</v>
+        <v>6244</v>
+      </c>
+      <c r="B6215" s="1">
+        <v>4398.4790599999997</v>
       </c>
     </row>
     <row r="6216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6216" t="s">
-        <v>6244</v>
+        <v>6245</v>
+      </c>
+      <c r="B6216" s="1">
+        <v>4411.3394399999997</v>
+      </c>
+    </row>
+    <row r="6217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6217" t="s">
+        <v>6246</v>
+      </c>
+    </row>
+    <row r="6218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6218" t="s">
+        <v>6246</v>
+      </c>
+    </row>
+    <row r="6219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6219" t="s">
+        <v>6247</v>
       </c>
     </row>
   </sheetData>
@@ -68919,19 +68952,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6245</v>
+        <v>6248</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6246</v>
+        <v>6249</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6247</v>
+        <v>6250</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6248</v>
+        <v>6251</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6249</v>
+        <v>6252</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68942,13 +68975,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68959,13 +68992,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68976,13 +69009,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68993,13 +69026,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69010,13 +69043,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69027,13 +69060,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69044,13 +69077,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69061,13 +69094,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69078,13 +69111,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69095,13 +69128,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69112,13 +69145,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69129,13 +69162,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69146,13 +69179,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69163,13 +69196,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69180,13 +69213,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6250</v>
+        <v>6253</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6251</v>
+        <v>6254</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6252</v>
+        <v>6255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de dados 01/12/2025
Atualização de dados 01/12/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42854D83-0AB9-41EB-A25F-2A38528B3DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7624768-C2AE-44F2-9162-22E0A8DA37BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6301" uniqueCount="6256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6305" uniqueCount="6260">
   <si>
     <t>Fecha</t>
   </si>
@@ -18756,10 +18756,22 @@
     <t>2025/11/26</t>
   </si>
   <si>
+    <t>2025/11/27</t>
+  </si>
+  <si>
+    <t>2025/11/28</t>
+  </si>
+  <si>
+    <t>2025/11/29</t>
+  </si>
+  <si>
+    <t>2025/11/30</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República jueves, 27 de noviembre de 2025 7:08:35 a. m.</t>
+    <t>Descargado de sistema del Banco de la República lunes, 1 de diciembre de 2025 9:02:30 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19175,10 +19187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6219"/>
+  <dimension ref="A1:B6223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F9" sqref="F8:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68918,15 +68930,47 @@
       <c r="A6217" t="s">
         <v>6246</v>
       </c>
+      <c r="B6217" s="1">
+        <v>4375.3005199999998</v>
+      </c>
     </row>
     <row r="6218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6218" t="s">
-        <v>6246</v>
+        <v>6247</v>
+      </c>
+      <c r="B6218" s="1">
+        <v>4379.4514799999997</v>
       </c>
     </row>
     <row r="6219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6219" t="s">
-        <v>6247</v>
+        <v>6248</v>
+      </c>
+      <c r="B6219" s="1">
+        <v>4345.5982299999996</v>
+      </c>
+    </row>
+    <row r="6220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6220" t="s">
+        <v>6249</v>
+      </c>
+      <c r="B6220" s="1">
+        <v>4345.5982299999996</v>
+      </c>
+    </row>
+    <row r="6221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6221" t="s">
+        <v>6250</v>
+      </c>
+    </row>
+    <row r="6222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6222" t="s">
+        <v>6250</v>
+      </c>
+    </row>
+    <row r="6223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6223" t="s">
+        <v>6251</v>
       </c>
     </row>
   </sheetData>
@@ -68952,19 +68996,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6248</v>
+        <v>6252</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6249</v>
+        <v>6253</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6250</v>
+        <v>6254</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6251</v>
+        <v>6255</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6252</v>
+        <v>6256</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68975,13 +69019,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -68992,13 +69036,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69009,13 +69053,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69026,13 +69070,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69043,13 +69087,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69060,13 +69104,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69077,13 +69121,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69094,13 +69138,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69111,13 +69155,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69128,13 +69172,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69145,13 +69189,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69162,13 +69206,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69179,13 +69223,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69196,13 +69240,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69213,13 +69257,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6253</v>
+        <v>6257</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6254</v>
+        <v>6258</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6255</v>
+        <v>6259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de dados 03/12/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7624768-C2AE-44F2-9162-22E0A8DA37BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F329C60-0104-4EEA-8EB7-23B5BCC0EFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6305" uniqueCount="6260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6307" uniqueCount="6262">
   <si>
     <t>Fecha</t>
   </si>
@@ -18768,10 +18768,16 @@
     <t>2025/11/30</t>
   </si>
   <si>
+    <t>2025/12/01</t>
+  </si>
+  <si>
+    <t>2025/12/02</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República lunes, 1 de diciembre de 2025 9:02:30 a. m.</t>
+    <t>Descargado de sistema del Banco de la República miércoles, 3 de diciembre de 2025 8:46:48 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19187,10 +19193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6223"/>
+  <dimension ref="A1:B6225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F8:F9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68962,15 +68968,31 @@
       <c r="A6221" t="s">
         <v>6250</v>
       </c>
+      <c r="B6221" s="1">
+        <v>4354.7720900000004</v>
+      </c>
     </row>
     <row r="6222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6222" t="s">
-        <v>6250</v>
+        <v>6251</v>
+      </c>
+      <c r="B6222" s="1">
+        <v>4392.3986699999996</v>
       </c>
     </row>
     <row r="6223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6223" t="s">
-        <v>6251</v>
+        <v>6252</v>
+      </c>
+    </row>
+    <row r="6224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6224" t="s">
+        <v>6252</v>
+      </c>
+    </row>
+    <row r="6225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6225" t="s">
+        <v>6253</v>
       </c>
     </row>
   </sheetData>
@@ -68996,19 +69018,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6252</v>
+        <v>6254</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6253</v>
+        <v>6255</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6254</v>
+        <v>6256</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6255</v>
+        <v>6257</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6256</v>
+        <v>6258</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69019,13 +69041,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69036,13 +69058,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69053,13 +69075,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69070,13 +69092,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69087,13 +69109,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69104,13 +69126,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69121,13 +69143,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69138,13 +69160,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69155,13 +69177,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69172,13 +69194,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69189,13 +69211,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69206,13 +69228,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69223,13 +69245,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69240,13 +69262,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69257,13 +69279,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de dados 05/12/2025
Atualização de dados 05/12/2025
</commit_message>
<xml_diff>
--- a/data/tasa_eur.xlsx
+++ b/data/tasa_eur.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F329C60-0104-4EEA-8EB7-23B5BCC0EFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1104B255-5641-4038-9F59-63282CDB159E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6307" uniqueCount="6262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6309" uniqueCount="6264">
   <si>
     <t>Fecha</t>
   </si>
@@ -18774,10 +18774,16 @@
     <t>2025/12/02</t>
   </si>
   <si>
+    <t>2025/12/03</t>
+  </si>
+  <si>
+    <t>2025/12/04</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Descargado de sistema del Banco de la República miércoles, 3 de diciembre de 2025 8:46:48 a. m.</t>
+    <t>Descargado de sistema del Banco de la República viernes, 5 de diciembre de 2025 8:29:13 a. m.</t>
   </si>
   <si>
     <t>Nombre de la serie</t>
@@ -19193,10 +19199,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6225"/>
+  <dimension ref="A1:B6227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68984,15 +68990,31 @@
       <c r="A6223" t="s">
         <v>6252</v>
       </c>
+      <c r="B6223" s="1">
+        <v>4451.9642000000003</v>
+      </c>
     </row>
     <row r="6224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6224" t="s">
-        <v>6252</v>
+        <v>6253</v>
+      </c>
+      <c r="B6224" s="1">
+        <v>4413.5168800000001</v>
       </c>
     </row>
     <row r="6225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6225" t="s">
-        <v>6253</v>
+        <v>6254</v>
+      </c>
+    </row>
+    <row r="6226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6226" t="s">
+        <v>6254</v>
+      </c>
+    </row>
+    <row r="6227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6227" t="s">
+        <v>6255</v>
       </c>
     </row>
   </sheetData>
@@ -69018,19 +69040,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6254</v>
+        <v>6256</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6255</v>
+        <v>6257</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6256</v>
+        <v>6258</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6258</v>
+        <v>6260</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69041,13 +69063,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69058,13 +69080,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69075,13 +69097,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69092,13 +69114,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69109,13 +69131,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69126,13 +69148,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69143,13 +69165,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69160,13 +69182,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69177,13 +69199,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69194,13 +69216,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69211,13 +69233,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69228,13 +69250,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69245,13 +69267,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69262,13 +69284,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
@@ -69279,13 +69301,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6259</v>
+        <v>6261</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6260</v>
+        <v>6262</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6261</v>
+        <v>6263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>